<commit_message>
Published state of ETDataset on 22 November 2017
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/transport/transport_car_using_compressed_natural_gas.converter.xlsx
+++ b/nodes_source_analyses/transport/transport_car_using_compressed_natural_gas.converter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorinevandervlies/Projects/etdataset/nodes_source_analyses/transport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/nodes_source_analyses/transport/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="460" windowWidth="19200" windowHeight="17540" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="9600" yWindow="460" windowWidth="19200" windowHeight="16240" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
   <si>
     <t>Source</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fixed operational and maintenance </t>
-  </si>
-  <si>
-    <t>output.car_kms</t>
   </si>
   <si>
     <t xml:space="preserve">Technical lifetime </t>
@@ -326,6 +323,45 @@
   <si>
     <t xml:space="preserve">This sheet summarizes all node attributes formatted in the way they are used by the Energy Transition Model. Use the Excel formulas to find the original data and sources for these numbers. You can also use this document to update the attribute value. Once you have finished updating, save this document and run rake import:node NODE="nodename" to update the node attributes on ETSource. 
 </t>
+  </si>
+  <si>
+    <t>CBS</t>
+  </si>
+  <si>
+    <t>vehicle km</t>
+  </si>
+  <si>
+    <t>mln vehicle km</t>
+  </si>
+  <si>
+    <t>passenger km</t>
+  </si>
+  <si>
+    <t>mld passenger km</t>
+  </si>
+  <si>
+    <t>passenger km/vehicle km</t>
+  </si>
+  <si>
+    <t>output.passenger_kms</t>
+  </si>
+  <si>
+    <t>pkm/MJ</t>
+  </si>
+  <si>
+    <t>Vehicle kilometers cars</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>http://statline.cbs.nl/Statweb/publication/?DM=SLNL&amp;PA=80302NED&amp;D1=a&amp;D2=a&amp;D3=25&amp;HDR=T,G2&amp;STB=G1&amp;VW=T</t>
+  </si>
+  <si>
+    <t>Passenger kilometers cars</t>
+  </si>
+  <si>
+    <t>http://statline.cbs.nl/Statweb/publication/?DM=SLNL&amp;PA=83497ned&amp;D1=0&amp;D2=a&amp;D3=0&amp;D4=5&amp;HDR=T,G3&amp;STB=G1,G2&amp;VW=T</t>
   </si>
 </sst>
 </file>
@@ -489,6 +525,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -496,6 +533,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -503,6 +541,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -510,17 +549,20 @@
       <sz val="16"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -528,16 +570,19 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1085,7 +1130,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1182,14 +1227,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="25" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1205,24 +1249,24 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1232,7 +1276,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1240,22 +1284,16 @@
     <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1263,17 +1301,30 @@
     <xf numFmtId="14" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1587,8 +1638,8 @@
       <xdr:rowOff>141116</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -1741,7 +1792,7 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>123</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1766,6 +1817,196 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>94967</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5016500" y="25113967"/>
+          <a:ext cx="5067300" cy="2279933"/>
+          <a:chOff x="9231573" y="32137067"/>
+          <a:chExt cx="12902777" cy="4417646"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="8" name="Picture 7"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9231573" y="32137067"/>
+            <a:ext cx="12902777" cy="4417646"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="13195110" y="34022352"/>
+            <a:ext cx="1173708" cy="552735"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>596899</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Group 9"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4838700" y="27673300"/>
+          <a:ext cx="10998199" cy="2514600"/>
+          <a:chOff x="9702800" y="37896800"/>
+          <a:chExt cx="16776701" cy="4152900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="11" name="Picture 10"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9702800" y="37896800"/>
+            <a:ext cx="16776701" cy="4152900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Rectangle 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="13367223" y="40003862"/>
+            <a:ext cx="1654792" cy="368490"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2215,10 +2456,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="18"/>
+    <col min="1" max="1" width="3.1640625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
@@ -2244,16 +2485,16 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2277,106 +2518,106 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="81"/>
+      <c r="B9" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="80"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="82"/>
-      <c r="C10" s="83"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="82"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="83" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="84" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="82"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="85" t="s">
-        <v>38</v>
+      <c r="B13" s="81"/>
+      <c r="C13" s="84" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="83" t="s">
-        <v>39</v>
+      <c r="B14" s="81"/>
+      <c r="C14" s="82" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="83"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="82"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="85" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="86" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="87" t="s">
-        <v>42</v>
+      <c r="B17" s="81"/>
+      <c r="C17" s="86" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="88" t="s">
-        <v>43</v>
+      <c r="B18" s="81"/>
+      <c r="C18" s="87" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="89" t="s">
-        <v>44</v>
+      <c r="B19" s="81"/>
+      <c r="C19" s="88" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="91" t="s">
-        <v>45</v>
+      <c r="B20" s="89"/>
+      <c r="C20" s="90" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="90"/>
-      <c r="C21" s="92" t="s">
-        <v>46</v>
+      <c r="B21" s="89"/>
+      <c r="C21" s="91" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="93" t="s">
+      <c r="B22" s="89"/>
+      <c r="C22" s="92" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="89"/>
+      <c r="C23" s="93" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="90"/>
-      <c r="C23" s="94" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2393,22 +2634,22 @@
   <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="32" customWidth="1"/>
-    <col min="2" max="2" width="2.28515625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="32" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="32" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" style="32" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="32" customWidth="1"/>
-    <col min="9" max="9" width="42.42578125" style="32" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="32" customWidth="1"/>
-    <col min="11" max="16384" width="10.7109375" style="32"/>
+    <col min="1" max="1" width="3.83203125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="2.33203125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="32" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="32" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="32" customWidth="1"/>
+    <col min="7" max="7" width="34.5" style="32" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" style="32" customWidth="1"/>
+    <col min="9" max="9" width="42.5" style="32" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="32" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
@@ -2418,38 +2659,38 @@
       <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="132" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="134"/>
+      <c r="B2" s="138" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="140"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="135"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="137"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="143"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="137"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="143"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="138"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="140"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="146"/>
     </row>
     <row r="6" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D6" s="33"/>
@@ -2473,7 +2714,7 @@
       <c r="D8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="101" t="s">
+      <c r="E8" s="100" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="15"/>
@@ -2484,7 +2725,7 @@
       <c r="I8" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="104"/>
+      <c r="J8" s="103"/>
     </row>
     <row r="9" spans="2:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="21"/>
@@ -2500,7 +2741,7 @@
     <row r="10" spans="2:10" s="22" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="13"/>
@@ -2512,49 +2753,49 @@
     </row>
     <row r="11" spans="2:10" s="22" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
-      <c r="C11" s="62" t="s">
-        <v>27</v>
+      <c r="C11" s="133" t="s">
+        <v>86</v>
       </c>
       <c r="D11" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="116">
+        <f>'Research data'!H7</f>
+        <v>0.63211786809616832</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="119">
-        <f>'Research data'!H7</f>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="116" t="s">
-        <v>71</v>
-      </c>
       <c r="H11" s="28"/>
-      <c r="I11" s="131" t="s">
-        <v>79</v>
+      <c r="I11" s="128" t="s">
+        <v>78</v>
       </c>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="37"/>
       <c r="C12" s="33"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="103"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="102"/>
       <c r="F12" s="33"/>
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="105"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="104"/>
     </row>
     <row r="13" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="37"/>
       <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="102"/>
-      <c r="E13" s="103"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="102"/>
       <c r="F13" s="33"/>
       <c r="G13" s="33"/>
       <c r="H13" s="33"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="105"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="104"/>
     </row>
     <row r="14" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="37"/>
@@ -2569,14 +2810,14 @@
         <v>15</v>
       </c>
       <c r="F14" s="36"/>
-      <c r="G14" s="68" t="s">
-        <v>28</v>
+      <c r="G14" s="67" t="s">
+        <v>27</v>
       </c>
       <c r="H14" s="36"/>
-      <c r="I14" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="105"/>
+      <c r="I14" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="104"/>
     </row>
     <row r="15" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="37"/>
@@ -2595,7 +2836,7 @@
       <c r="I15" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="105"/>
+      <c r="J15" s="104"/>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
@@ -2626,28 +2867,28 @@
   <dimension ref="B2:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="42" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="42" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="42" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="42" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="42" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="42" customWidth="1"/>
-    <col min="7" max="7" width="3.140625" style="42" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="42" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" style="42" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="42" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" style="42" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="42" customWidth="1"/>
-    <col min="13" max="13" width="2.28515625" style="42" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" style="42" customWidth="1"/>
-    <col min="15" max="15" width="2.42578125" style="42" customWidth="1"/>
-    <col min="16" max="16" width="68.85546875" style="42" customWidth="1"/>
-    <col min="17" max="16384" width="10.7109375" style="42"/>
+    <col min="1" max="1" width="3.33203125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="42" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="42" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="42" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="42" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="42" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" style="42" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="42" customWidth="1"/>
+    <col min="9" max="9" width="2.5" style="42" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="42" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" style="42" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="42" customWidth="1"/>
+    <col min="13" max="13" width="2.33203125" style="42" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="42" customWidth="1"/>
+    <col min="15" max="15" width="2.5" style="42" customWidth="1"/>
+    <col min="16" max="16" width="68.83203125" style="42" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="42"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2670,33 +2911,33 @@
     </row>
     <row r="4" spans="2:16" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="21"/>
-      <c r="C4" s="97" t="s">
-        <v>52</v>
+      <c r="C4" s="96" t="s">
+        <v>51</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97" t="s">
+      <c r="G4" s="96"/>
+      <c r="H4" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="96"/>
+      <c r="P4" s="96" t="s">
         <v>56</v>
-      </c>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97" t="s">
-        <v>74</v>
-      </c>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2716,7 +2957,7 @@
     <row r="6" spans="2:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="45"/>
       <c r="C6" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -2734,32 +2975,32 @@
     </row>
     <row r="7" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45"/>
-      <c r="C7" s="114" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="115" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="98"/>
-      <c r="H7" s="118">
+      <c r="C7" s="134" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="135" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="97"/>
+      <c r="H7" s="115">
         <f>N7</f>
-        <v>0.47619047619047616</v>
+        <v>0.63211786809616832</v>
       </c>
       <c r="I7" s="49"/>
-      <c r="J7" s="118">
-        <f>Notes!D28</f>
-        <v>0.45454545454545453</v>
+      <c r="J7" s="115">
+        <f>Notes!E131</f>
+        <v>0.60338523772816066</v>
       </c>
       <c r="K7" s="46"/>
-      <c r="N7" s="118">
-        <f>Notes!D82</f>
-        <v>0.47619047619047616</v>
+      <c r="N7" s="115">
+        <f>Notes!D83</f>
+        <v>0.63211786809616832</v>
       </c>
       <c r="O7" s="46"/>
-      <c r="P7" s="130" t="s">
-        <v>78</v>
+      <c r="P7" s="127" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
@@ -2805,7 +3046,7 @@
       <c r="F10" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="98"/>
+      <c r="G10" s="97"/>
       <c r="H10" s="53">
         <f>ROUND(15,0)</f>
         <v>15</v>
@@ -2842,7 +3083,7 @@
     <row r="12" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="45"/>
       <c r="C12" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -2856,19 +3097,19 @@
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
       <c r="O12" s="46"/>
-      <c r="P12" s="69"/>
+      <c r="P12" s="68"/>
     </row>
     <row r="13" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="45"/>
       <c r="C13" s="52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="99"/>
+      <c r="G13" s="98"/>
       <c r="H13" s="50">
         <f>ROUND(18300,2)</f>
         <v>18300</v>
@@ -2883,19 +3124,19 @@
       <c r="M13" s="49"/>
       <c r="N13" s="49"/>
       <c r="O13" s="49"/>
-      <c r="P13" s="96"/>
+      <c r="P13" s="95"/>
     </row>
     <row r="14" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="45"/>
       <c r="C14" s="52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="54"/>
       <c r="E14" s="54"/>
-      <c r="F14" s="95" t="s">
+      <c r="F14" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="100"/>
+      <c r="G14" s="99"/>
       <c r="H14" s="55">
         <f>ROUND(482.4,2)</f>
         <v>482.4</v>
@@ -2910,8 +3151,8 @@
       <c r="M14" s="49"/>
       <c r="N14" s="49"/>
       <c r="O14" s="49"/>
-      <c r="P14" s="113" t="s">
-        <v>69</v>
+      <c r="P14" s="112" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2925,250 +3166,310 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="63" customWidth="1"/>
-    <col min="2" max="2" width="2.140625" style="63" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="63" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="63" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="63" customWidth="1"/>
-    <col min="6" max="7" width="13.28515625" style="63" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="70" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" style="70" customWidth="1"/>
-    <col min="10" max="10" width="98.42578125" style="63" customWidth="1"/>
-    <col min="11" max="16384" width="33.140625" style="63"/>
+    <col min="1" max="1" width="5.5" style="62" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="62" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="62" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="62" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" style="62" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="69" customWidth="1"/>
+    <col min="9" max="9" width="34.5" style="69" customWidth="1"/>
+    <col min="10" max="10" width="98.5" style="62" customWidth="1"/>
+    <col min="11" max="16384" width="33.1640625" style="62"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="65"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="64"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="66"/>
-      <c r="C3" s="72" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="67"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="67"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="75"/>
-      <c r="C5" s="76" t="s">
+      <c r="B5" s="74"/>
+      <c r="C5" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="76" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="77" t="s">
+      <c r="G5" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="77" t="s">
+      <c r="I5" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="65"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="71"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="65"/>
+      <c r="C7" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="66">
+        <v>2013</v>
+      </c>
+      <c r="G7" s="66">
+        <v>2012</v>
+      </c>
+      <c r="H7" s="117">
+        <v>42326</v>
+      </c>
+      <c r="I7" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="76" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="66"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="72"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="66"/>
-      <c r="C7" s="79" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="67" t="s">
+      <c r="J7" s="66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="65"/>
+      <c r="C8" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="65"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="65"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="65"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="66">
+        <v>2011</v>
+      </c>
+      <c r="G11" s="66">
+        <v>2011</v>
+      </c>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="66" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="65"/>
+      <c r="C12" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="65"/>
+      <c r="C13" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="120"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="122"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="120"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="125" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="67">
-        <v>2013</v>
-      </c>
-      <c r="G7" s="67">
-        <v>2012</v>
-      </c>
-      <c r="H7" s="120">
+      <c r="F15" s="123">
+        <v>2014</v>
+      </c>
+      <c r="G15" s="123">
+        <v>2014</v>
+      </c>
+      <c r="H15" s="126">
         <v>42326</v>
       </c>
-      <c r="I7" s="67" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="67" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="66"/>
-      <c r="C8" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="66"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="66"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="66"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="67">
-        <v>2011</v>
-      </c>
-      <c r="G11" s="67">
-        <v>2011</v>
-      </c>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="67" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="66"/>
-      <c r="C12" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="66"/>
-      <c r="C13" s="78" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="123"/>
-      <c r="B14" s="124"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="123"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="126"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="128" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="126" t="s">
+      <c r="I15" s="123" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="124"/>
+      <c r="C16" s="125"/>
+    </row>
+    <row r="17" spans="2:10" s="136" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="124"/>
+      <c r="C17" s="125" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="136" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="126">
-        <v>2014</v>
-      </c>
-      <c r="G15" s="126">
-        <v>2014</v>
-      </c>
-      <c r="H15" s="129">
-        <v>42326</v>
-      </c>
-      <c r="I15" s="126" t="s">
-        <v>76</v>
-      </c>
-      <c r="J15" s="63" t="s">
-        <v>77</v>
-      </c>
+      <c r="G17" s="136">
+        <v>2015</v>
+      </c>
+      <c r="H17" s="137" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="137"/>
+      <c r="J17" s="136" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" s="136" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="124"/>
+      <c r="C18" s="125"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="137"/>
+    </row>
+    <row r="19" spans="2:10" s="136" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="124"/>
+      <c r="C19" s="125" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="136" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="136" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="136">
+        <v>2015</v>
+      </c>
+      <c r="H19" s="137" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="137"/>
+      <c r="J19" s="136" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="124"/>
+      <c r="C20" s="125"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3178,985 +3479,1247 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M117"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="106" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="106" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="106"/>
-    <col min="4" max="4" width="8.42578125" style="106" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="106"/>
+    <col min="1" max="1" width="4.6640625" style="105" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="105" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="105"/>
+    <col min="4" max="4" width="8.5" style="105" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="105"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="107"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
     </row>
     <row r="3" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="111"/>
-      <c r="C3" s="101" t="s">
+      <c r="B3" s="110"/>
+      <c r="C3" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="101" t="s">
+      <c r="D3" s="100" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="108"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="108"/>
+      <c r="C5" s="109" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="109"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="108"/>
+      <c r="C6" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="109"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="110"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="109"/>
-      <c r="C5" s="110" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="110"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="109"/>
-      <c r="C6" s="110" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="109"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="110"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="109"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="109"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="110"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="109"/>
+      <c r="M8" s="109"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="109"/>
-      <c r="C9" s="110"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="110"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="109"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="109"/>
-      <c r="C10" s="110"/>
-      <c r="D10" s="110">
+      <c r="B10" s="108"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109">
         <v>18300</v>
       </c>
-      <c r="E10" s="110" t="s">
+      <c r="E10" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
-      <c r="K10" s="110"/>
-      <c r="L10" s="110"/>
-      <c r="M10" s="110"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
+      <c r="K10" s="109"/>
+      <c r="L10" s="109"/>
+      <c r="M10" s="109"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="109"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="110"/>
-      <c r="L11" s="110"/>
-      <c r="M11" s="110"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="109"/>
+      <c r="M11" s="109"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="109"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
-      <c r="K12" s="110"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="110"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="109"/>
+      <c r="M12" s="109"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="109"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
-      <c r="L13" s="110"/>
-      <c r="M13" s="110"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="109"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="109"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="110"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="109"/>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="110"/>
-      <c r="M15" s="110"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="109"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="109"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="110"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="110"/>
-      <c r="K16" s="110"/>
-      <c r="L16" s="110"/>
-      <c r="M16" s="110"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="109"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="109"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="109"/>
+      <c r="K16" s="109"/>
+      <c r="L16" s="109"/>
+      <c r="M16" s="109"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B17" s="109"/>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="110"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="110"/>
-      <c r="K17" s="110"/>
-      <c r="L17" s="110"/>
-      <c r="M17" s="110"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="109"/>
+      <c r="M17" s="109"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="109"/>
-      <c r="C18" s="110"/>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="110"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="110"/>
-      <c r="K18" s="110"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="110"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="109"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="110"/>
-      <c r="L19" s="110"/>
-      <c r="M19" s="110"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="109"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="110"/>
-      <c r="M20" s="110"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
+      <c r="G20" s="109"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="109"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B21" s="109"/>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="110"/>
-      <c r="L21" s="110"/>
-      <c r="M21" s="110"/>
+      <c r="B21" s="108"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="109"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="109"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="110"/>
-      <c r="M22" s="110"/>
+      <c r="B22" s="108"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="109"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="109"/>
+      <c r="M22" s="109"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B23" s="109"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="110"/>
-      <c r="L23" s="110"/>
-      <c r="M23" s="110"/>
+      <c r="B23" s="108"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="109"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B24" s="109"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="110"/>
-      <c r="K24" s="110"/>
-      <c r="L24" s="110"/>
-      <c r="M24" s="110"/>
+      <c r="B24" s="108"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
+      <c r="K24" s="109"/>
+      <c r="L24" s="109"/>
+      <c r="M24" s="109"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="109"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="110"/>
-      <c r="K25" s="110"/>
-      <c r="L25" s="110"/>
-      <c r="M25" s="110"/>
+      <c r="B25" s="108"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
+      <c r="J25" s="109"/>
+      <c r="K25" s="109"/>
+      <c r="L25" s="109"/>
+      <c r="M25" s="109"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="109"/>
-      <c r="C26" s="117" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="110"/>
-      <c r="G26" s="110"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="110"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="110"/>
-      <c r="L26" s="110"/>
-      <c r="M26" s="110"/>
+      <c r="B26" s="108"/>
+      <c r="C26" s="114" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="109"/>
+      <c r="G26" s="109"/>
+      <c r="H26" s="109"/>
+      <c r="I26" s="109"/>
+      <c r="J26" s="109"/>
+      <c r="K26" s="109"/>
+      <c r="L26" s="109"/>
+      <c r="M26" s="109"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="109"/>
-      <c r="D27" s="106">
+      <c r="B27" s="108"/>
+      <c r="D27" s="105">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E27" s="117" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="110"/>
+      <c r="E27" s="114" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109"/>
+      <c r="M27" s="109"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="109"/>
-      <c r="D28" s="106">
+      <c r="B28" s="108"/>
+      <c r="D28" s="105">
         <f>1/D27</f>
         <v>0.45454545454545453</v>
       </c>
-      <c r="E28" s="117" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="110"/>
-      <c r="G28" s="110"/>
-      <c r="H28" s="110"/>
-      <c r="I28" s="110"/>
-      <c r="J28" s="110"/>
-      <c r="K28" s="110"/>
-      <c r="L28" s="110"/>
-      <c r="M28" s="110"/>
+      <c r="E28" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
+      <c r="J28" s="109"/>
+      <c r="K28" s="109"/>
+      <c r="L28" s="109"/>
+      <c r="M28" s="109"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B29" s="109"/>
-      <c r="F29" s="110"/>
-      <c r="G29" s="110"/>
-      <c r="H29" s="110"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="110"/>
-      <c r="L29" s="110"/>
-      <c r="M29" s="110"/>
+      <c r="B29" s="108"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="109"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="109"/>
+      <c r="J29" s="109"/>
+      <c r="K29" s="109"/>
+      <c r="L29" s="109"/>
+      <c r="M29" s="109"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="109"/>
-      <c r="F30" s="110"/>
-      <c r="G30" s="110"/>
-      <c r="H30" s="110"/>
-      <c r="I30" s="110"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="110"/>
-      <c r="L30" s="110"/>
-      <c r="M30" s="110"/>
+      <c r="B30" s="108"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="109"/>
+      <c r="H30" s="109"/>
+      <c r="I30" s="109"/>
+      <c r="J30" s="109"/>
+      <c r="K30" s="109"/>
+      <c r="L30" s="109"/>
+      <c r="M30" s="109"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B31" s="109"/>
-      <c r="F31" s="110"/>
-      <c r="G31" s="110"/>
-      <c r="H31" s="110"/>
-      <c r="I31" s="110"/>
-      <c r="J31" s="110"/>
-      <c r="K31" s="110"/>
-      <c r="L31" s="110"/>
-      <c r="M31" s="110"/>
+      <c r="B31" s="108"/>
+      <c r="F31" s="109"/>
+      <c r="G31" s="109"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="109"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="109"/>
+      <c r="M31" s="109"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B32" s="109"/>
-      <c r="F32" s="110"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="110"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="110"/>
-      <c r="K32" s="110"/>
-      <c r="L32" s="110"/>
-      <c r="M32" s="110"/>
+      <c r="B32" s="108"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="109"/>
+      <c r="J32" s="109"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="109"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B33" s="109"/>
-      <c r="F33" s="110"/>
-      <c r="G33" s="110"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="110"/>
-      <c r="J33" s="110"/>
-      <c r="K33" s="110"/>
-      <c r="L33" s="110"/>
-      <c r="M33" s="110"/>
+      <c r="B33" s="108"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="109"/>
+      <c r="J33" s="109"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="109"/>
+      <c r="M33" s="109"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B34" s="109"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110"/>
-      <c r="K34" s="110"/>
-      <c r="L34" s="110"/>
-      <c r="M34" s="110"/>
+      <c r="B34" s="108"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="109"/>
+      <c r="M34" s="109"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B35" s="109"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="110"/>
-      <c r="J35" s="110"/>
-      <c r="K35" s="110"/>
-      <c r="L35" s="110"/>
-      <c r="M35" s="110"/>
+      <c r="B35" s="108"/>
+      <c r="F35" s="109"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="109"/>
+      <c r="J35" s="109"/>
+      <c r="K35" s="109"/>
+      <c r="L35" s="109"/>
+      <c r="M35" s="109"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B36" s="109"/>
-      <c r="F36" s="110"/>
-      <c r="G36" s="110"/>
-      <c r="H36" s="110"/>
-      <c r="I36" s="110"/>
-      <c r="J36" s="110"/>
-      <c r="K36" s="110"/>
-      <c r="L36" s="110"/>
-      <c r="M36" s="110"/>
+      <c r="B36" s="108"/>
+      <c r="F36" s="109"/>
+      <c r="G36" s="109"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="109"/>
+      <c r="J36" s="109"/>
+      <c r="K36" s="109"/>
+      <c r="L36" s="109"/>
+      <c r="M36" s="109"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B37" s="109"/>
-      <c r="C37" s="110"/>
-      <c r="D37" s="110"/>
-      <c r="E37" s="110"/>
-      <c r="F37" s="110"/>
-      <c r="G37" s="110"/>
-      <c r="H37" s="110"/>
-      <c r="I37" s="110"/>
-      <c r="J37" s="110"/>
-      <c r="K37" s="110"/>
-      <c r="L37" s="110"/>
-      <c r="M37" s="110"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="109"/>
+      <c r="E37" s="109"/>
+      <c r="F37" s="109"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="109"/>
+      <c r="J37" s="109"/>
+      <c r="K37" s="109"/>
+      <c r="L37" s="109"/>
+      <c r="M37" s="109"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="109"/>
-      <c r="C38" s="110"/>
-      <c r="D38" s="110"/>
-      <c r="E38" s="110"/>
-      <c r="F38" s="110"/>
-      <c r="G38" s="110"/>
-      <c r="H38" s="110"/>
-      <c r="I38" s="110"/>
-      <c r="J38" s="110"/>
-      <c r="K38" s="110"/>
-      <c r="L38" s="110"/>
-      <c r="M38" s="110"/>
+      <c r="B38" s="108"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="109"/>
+      <c r="G38" s="109"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="109"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="109"/>
+      <c r="M38" s="109"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B39" s="109"/>
-      <c r="C39" s="110" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="110"/>
-      <c r="E39" s="110"/>
-      <c r="F39" s="110"/>
-      <c r="G39" s="110"/>
-      <c r="H39" s="110"/>
-      <c r="I39" s="110"/>
-      <c r="J39" s="110"/>
-      <c r="K39" s="110"/>
-      <c r="L39" s="110"/>
-      <c r="M39" s="110"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="109" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="109"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="109"/>
+      <c r="G39" s="109"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="109"/>
+      <c r="J39" s="109"/>
+      <c r="K39" s="109"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B40" s="109"/>
-      <c r="C40" s="110" t="s">
+      <c r="B40" s="108"/>
+      <c r="C40" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="109"/>
+      <c r="E40" s="109"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="109"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="109"/>
+      <c r="J40" s="109"/>
+      <c r="K40" s="109"/>
+      <c r="L40" s="109"/>
+      <c r="M40" s="109"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B41" s="108"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
+      <c r="F41" s="109"/>
+      <c r="G41" s="109"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="109"/>
+      <c r="J41" s="109"/>
+      <c r="K41" s="109"/>
+      <c r="L41" s="109"/>
+      <c r="M41" s="109"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B42" s="108"/>
+      <c r="C42" s="109"/>
+      <c r="D42" s="109"/>
+      <c r="E42" s="109"/>
+      <c r="F42" s="109"/>
+      <c r="G42" s="109"/>
+      <c r="H42" s="109"/>
+      <c r="I42" s="109"/>
+      <c r="J42" s="109"/>
+      <c r="K42" s="109"/>
+      <c r="L42" s="109"/>
+      <c r="M42" s="109"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" s="108"/>
+      <c r="C43" s="109"/>
+      <c r="D43" s="109">
+        <v>15</v>
+      </c>
+      <c r="E43" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="110"/>
-      <c r="E40" s="110"/>
-      <c r="F40" s="110"/>
-      <c r="G40" s="110"/>
-      <c r="H40" s="110"/>
-      <c r="I40" s="110"/>
-      <c r="J40" s="110"/>
-      <c r="K40" s="110"/>
-      <c r="L40" s="110"/>
-      <c r="M40" s="110"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B41" s="109"/>
-      <c r="C41" s="110"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="110"/>
-      <c r="F41" s="110"/>
-      <c r="G41" s="110"/>
-      <c r="H41" s="110"/>
-      <c r="I41" s="110"/>
-      <c r="J41" s="110"/>
-      <c r="K41" s="110"/>
-      <c r="L41" s="110"/>
-      <c r="M41" s="110"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B42" s="109"/>
-      <c r="C42" s="110"/>
-      <c r="D42" s="110"/>
-      <c r="E42" s="110"/>
-      <c r="F42" s="110"/>
-      <c r="G42" s="110"/>
-      <c r="H42" s="110"/>
-      <c r="I42" s="110"/>
-      <c r="J42" s="110"/>
-      <c r="K42" s="110"/>
-      <c r="L42" s="110"/>
-      <c r="M42" s="110"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B43" s="109"/>
-      <c r="C43" s="110"/>
-      <c r="D43" s="110">
-        <v>15</v>
-      </c>
-      <c r="E43" s="110" t="s">
+      <c r="F43" s="109"/>
+      <c r="G43" s="109"/>
+      <c r="H43" s="109"/>
+      <c r="I43" s="109"/>
+      <c r="J43" s="109"/>
+      <c r="K43" s="109"/>
+      <c r="L43" s="109"/>
+      <c r="M43" s="109"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" s="108"/>
+      <c r="C44" s="109"/>
+      <c r="D44" s="109"/>
+      <c r="E44" s="109"/>
+      <c r="F44" s="109"/>
+      <c r="G44" s="109"/>
+      <c r="H44" s="109"/>
+      <c r="I44" s="109"/>
+      <c r="J44" s="109"/>
+      <c r="K44" s="109"/>
+      <c r="L44" s="109"/>
+      <c r="M44" s="109"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" s="108"/>
+      <c r="C45" s="109"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="109"/>
+      <c r="F45" s="109"/>
+      <c r="G45" s="109"/>
+      <c r="H45" s="109"/>
+      <c r="I45" s="109"/>
+      <c r="J45" s="109"/>
+      <c r="K45" s="109"/>
+      <c r="L45" s="109"/>
+      <c r="M45" s="109"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B46" s="108"/>
+      <c r="C46" s="109"/>
+      <c r="D46" s="109"/>
+      <c r="E46" s="109"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
+      <c r="H46" s="109"/>
+      <c r="I46" s="109"/>
+      <c r="J46" s="109"/>
+      <c r="K46" s="109"/>
+      <c r="L46" s="109"/>
+      <c r="M46" s="109"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B47" s="108"/>
+      <c r="C47" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="110"/>
-      <c r="G43" s="110"/>
-      <c r="H43" s="110"/>
-      <c r="I43" s="110"/>
-      <c r="J43" s="110"/>
-      <c r="K43" s="110"/>
-      <c r="L43" s="110"/>
-      <c r="M43" s="110"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B44" s="109"/>
-      <c r="C44" s="110"/>
-      <c r="D44" s="110"/>
-      <c r="E44" s="110"/>
-      <c r="F44" s="110"/>
-      <c r="G44" s="110"/>
-      <c r="H44" s="110"/>
-      <c r="I44" s="110"/>
-      <c r="J44" s="110"/>
-      <c r="K44" s="110"/>
-      <c r="L44" s="110"/>
-      <c r="M44" s="110"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B45" s="109"/>
-      <c r="C45" s="110"/>
-      <c r="D45" s="110"/>
-      <c r="E45" s="110"/>
-      <c r="F45" s="110"/>
-      <c r="G45" s="110"/>
-      <c r="H45" s="110"/>
-      <c r="I45" s="110"/>
-      <c r="J45" s="110"/>
-      <c r="K45" s="110"/>
-      <c r="L45" s="110"/>
-      <c r="M45" s="110"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B46" s="109"/>
-      <c r="C46" s="110"/>
-      <c r="D46" s="110"/>
-      <c r="E46" s="110"/>
-      <c r="F46" s="110"/>
-      <c r="G46" s="110"/>
-      <c r="H46" s="110"/>
-      <c r="I46" s="110"/>
-      <c r="J46" s="110"/>
-      <c r="K46" s="110"/>
-      <c r="L46" s="110"/>
-      <c r="M46" s="110"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="109"/>
-      <c r="C47" s="110" t="s">
+      <c r="D47" s="109"/>
+      <c r="E47" s="109"/>
+      <c r="F47" s="109"/>
+      <c r="G47" s="109"/>
+      <c r="H47" s="109"/>
+      <c r="I47" s="109"/>
+      <c r="J47" s="109"/>
+      <c r="K47" s="109"/>
+      <c r="L47" s="109"/>
+      <c r="M47" s="109"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" s="108"/>
+      <c r="C48" s="109"/>
+      <c r="D48" s="109"/>
+      <c r="E48" s="109"/>
+      <c r="F48" s="109"/>
+      <c r="G48" s="109"/>
+      <c r="H48" s="109"/>
+      <c r="I48" s="109"/>
+      <c r="J48" s="109"/>
+      <c r="K48" s="109"/>
+      <c r="L48" s="109"/>
+      <c r="M48" s="109"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B49" s="108"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="109"/>
+      <c r="E49" s="109"/>
+      <c r="F49" s="109"/>
+      <c r="G49" s="109"/>
+      <c r="H49" s="109"/>
+      <c r="I49" s="109"/>
+      <c r="J49" s="109"/>
+      <c r="K49" s="109"/>
+      <c r="L49" s="109"/>
+      <c r="M49" s="109"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B50" s="108"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="109"/>
+      <c r="E50" s="109"/>
+      <c r="F50" s="109"/>
+      <c r="G50" s="109"/>
+      <c r="H50" s="109"/>
+      <c r="I50" s="109"/>
+      <c r="J50" s="109"/>
+      <c r="K50" s="109"/>
+      <c r="L50" s="109"/>
+      <c r="M50" s="109"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" s="108"/>
+      <c r="C51" s="109"/>
+      <c r="D51" s="109"/>
+      <c r="E51" s="109"/>
+      <c r="F51" s="109"/>
+      <c r="G51" s="109"/>
+      <c r="H51" s="109"/>
+      <c r="I51" s="109"/>
+      <c r="J51" s="109"/>
+      <c r="K51" s="109"/>
+      <c r="L51" s="109"/>
+      <c r="M51" s="109"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52" s="108"/>
+      <c r="C52" s="109"/>
+      <c r="D52" s="109"/>
+      <c r="E52" s="109"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B53" s="108"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109">
+        <v>3321</v>
+      </c>
+      <c r="E53" s="111" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B54" s="108"/>
+      <c r="C54" s="109"/>
+      <c r="D54" s="109">
+        <v>2412</v>
+      </c>
+      <c r="E54" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="110"/>
-      <c r="E47" s="110"/>
-      <c r="F47" s="110"/>
-      <c r="G47" s="110"/>
-      <c r="H47" s="110"/>
-      <c r="I47" s="110"/>
-      <c r="J47" s="110"/>
-      <c r="K47" s="110"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="110"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="109"/>
-      <c r="C48" s="110"/>
-      <c r="D48" s="110"/>
-      <c r="E48" s="110"/>
-      <c r="F48" s="110"/>
-      <c r="G48" s="110"/>
-      <c r="H48" s="110"/>
-      <c r="I48" s="110"/>
-      <c r="J48" s="110"/>
-      <c r="K48" s="110"/>
-      <c r="L48" s="110"/>
-      <c r="M48" s="110"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B49" s="109"/>
-      <c r="C49" s="110"/>
-      <c r="D49" s="110"/>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B50" s="109"/>
-      <c r="C50" s="110"/>
-      <c r="D50" s="110"/>
-      <c r="E50" s="110"/>
-      <c r="F50" s="110"/>
-      <c r="G50" s="110"/>
-      <c r="H50" s="110"/>
-      <c r="I50" s="110"/>
-      <c r="J50" s="110"/>
-      <c r="K50" s="110"/>
-      <c r="L50" s="110"/>
-      <c r="M50" s="110"/>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B51" s="109"/>
-      <c r="C51" s="110"/>
-      <c r="D51" s="110"/>
-      <c r="E51" s="110"/>
-      <c r="F51" s="110"/>
-      <c r="G51" s="110"/>
-      <c r="H51" s="110"/>
-      <c r="I51" s="110"/>
-      <c r="J51" s="110"/>
-      <c r="K51" s="110"/>
-      <c r="L51" s="110"/>
-      <c r="M51" s="110"/>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B52" s="109"/>
-      <c r="C52" s="110"/>
-      <c r="D52" s="110"/>
-      <c r="E52" s="110"/>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B53" s="109"/>
-      <c r="C53" s="110"/>
-      <c r="D53" s="110">
-        <v>3321</v>
-      </c>
-      <c r="E53" s="112" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B54" s="109"/>
-      <c r="C54" s="110"/>
-      <c r="D54" s="110">
-        <v>2412</v>
-      </c>
-      <c r="E54" s="110" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B55" s="109"/>
+      <c r="B55" s="108"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B56" s="109"/>
+      <c r="B56" s="108"/>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B57" s="109"/>
+      <c r="B57" s="108"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B58" s="109"/>
+      <c r="B58" s="108"/>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B59" s="109"/>
+      <c r="B59" s="108"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B60" s="109"/>
+      <c r="B60" s="108"/>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B61" s="109"/>
+      <c r="B61" s="108"/>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B62" s="109"/>
+      <c r="B62" s="108"/>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B63" s="109"/>
+      <c r="B63" s="108"/>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B64" s="109"/>
+      <c r="B64" s="108"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B65" s="109"/>
+      <c r="B65" s="108"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B66" s="109"/>
+      <c r="B66" s="108"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B67" s="109"/>
+      <c r="B67" s="108"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B68" s="109"/>
+      <c r="B68" s="108"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B69" s="109"/>
+      <c r="B69" s="108"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B70" s="109"/>
-      <c r="C70" s="123" t="s">
+      <c r="B70" s="108"/>
+      <c r="C70" s="120" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B71" s="108"/>
+      <c r="C71" s="120" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B71" s="109"/>
-      <c r="C71" s="123" t="s">
-        <v>75</v>
-      </c>
-    </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B72" s="109"/>
+      <c r="B72" s="108"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B73" s="109"/>
+      <c r="B73" s="108"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B74" s="109"/>
+      <c r="B74" s="108"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B75" s="109"/>
+      <c r="B75" s="108"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B76" s="109"/>
+      <c r="B76" s="108"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B77" s="109"/>
+      <c r="B77" s="108"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="121"/>
-      <c r="B78" s="122"/>
+      <c r="A78" s="118"/>
+      <c r="B78" s="119"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="121"/>
-      <c r="B79" s="122"/>
+      <c r="A79" s="118"/>
+      <c r="B79" s="119"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="121"/>
-      <c r="B80" s="122"/>
+      <c r="A80" s="118"/>
+      <c r="B80" s="119"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="121"/>
-      <c r="B81" s="122"/>
-      <c r="D81" s="106">
+      <c r="A81" s="118"/>
+      <c r="B81" s="119"/>
+      <c r="D81" s="105">
         <v>2.1</v>
       </c>
-      <c r="E81" s="123" t="s">
-        <v>72</v>
+      <c r="E81" s="120" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="121"/>
-      <c r="B82" s="122"/>
-      <c r="D82" s="106">
+      <c r="A82" s="118"/>
+      <c r="B82" s="119"/>
+      <c r="D82" s="105">
         <f>1/D81</f>
         <v>0.47619047619047616</v>
       </c>
-      <c r="E82" s="123" t="s">
-        <v>70</v>
+      <c r="E82" s="120" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="121"/>
-      <c r="B83" s="122"/>
+      <c r="A83" s="118"/>
+      <c r="B83" s="119"/>
+      <c r="C83" s="62" t="str">
+        <f>'Research data'!C7</f>
+        <v>output.passenger_kms</v>
+      </c>
+      <c r="D83" s="62">
+        <f>E129*D82</f>
+        <v>0.63211786809616832</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="121"/>
-      <c r="B84" s="122"/>
+      <c r="A84" s="118"/>
+      <c r="B84" s="119"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="121"/>
-      <c r="B85" s="122"/>
+      <c r="A85" s="118"/>
+      <c r="B85" s="119"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="121"/>
-      <c r="B86" s="122"/>
+      <c r="A86" s="118"/>
+      <c r="B86" s="119"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="121"/>
-      <c r="B87" s="122"/>
+      <c r="A87" s="118"/>
+      <c r="B87" s="119"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="121"/>
-      <c r="B88" s="122"/>
+      <c r="A88" s="118"/>
+      <c r="B88" s="119"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="121"/>
-      <c r="B89" s="122"/>
+      <c r="A89" s="118"/>
+      <c r="B89" s="119"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="121"/>
-      <c r="B90" s="122"/>
+      <c r="A90" s="118"/>
+      <c r="B90" s="119"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="121"/>
-      <c r="B91" s="122"/>
+      <c r="A91" s="118"/>
+      <c r="B91" s="119"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="121"/>
-      <c r="B92" s="122"/>
+      <c r="A92" s="118"/>
+      <c r="B92" s="119"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="121"/>
-      <c r="B93" s="122"/>
+      <c r="A93" s="118"/>
+      <c r="B93" s="119"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="121"/>
-      <c r="B94" s="122"/>
+      <c r="A94" s="118"/>
+      <c r="B94" s="119"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="121"/>
-      <c r="B95" s="122"/>
+      <c r="A95" s="118"/>
+      <c r="B95" s="119"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="121"/>
-      <c r="B96" s="122"/>
+      <c r="A96" s="118"/>
+      <c r="B96" s="119"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="121"/>
-      <c r="B97" s="122"/>
+      <c r="A97" s="118"/>
+      <c r="B97" s="119"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="121"/>
-      <c r="B98" s="122"/>
+      <c r="A98" s="118"/>
+      <c r="B98" s="119"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="121"/>
-      <c r="B99" s="122"/>
+      <c r="A99" s="118"/>
+      <c r="B99" s="119"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="121"/>
-      <c r="B100" s="122"/>
+      <c r="A100" s="118"/>
+      <c r="B100" s="119"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="121"/>
-      <c r="B101" s="122"/>
+      <c r="A101" s="118"/>
+      <c r="B101" s="119"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="121"/>
-      <c r="B102" s="122"/>
+      <c r="A102" s="118"/>
+      <c r="B102" s="119"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="121"/>
-      <c r="B103" s="122"/>
+      <c r="A103" s="118"/>
+      <c r="B103" s="119"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="121"/>
-      <c r="B104" s="122"/>
+      <c r="A104" s="118"/>
+      <c r="B104" s="119"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="121"/>
-      <c r="B105" s="122"/>
+      <c r="A105" s="118"/>
+      <c r="B105" s="119"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="121"/>
-      <c r="B106" s="122"/>
+      <c r="A106" s="118"/>
+      <c r="B106" s="119"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="121"/>
-      <c r="B107" s="122"/>
+      <c r="A107" s="118"/>
+      <c r="B107" s="119"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="121"/>
-      <c r="B108" s="122"/>
+      <c r="A108" s="118"/>
+      <c r="B108" s="119"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="121"/>
-      <c r="B109" s="122"/>
+      <c r="A109" s="118"/>
+      <c r="B109" s="119"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="121"/>
-      <c r="B110" s="122"/>
+      <c r="A110" s="118"/>
+      <c r="B110" s="119"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="121"/>
-      <c r="B111" s="122"/>
+      <c r="A111" s="118"/>
+      <c r="B111" s="119"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="121"/>
-      <c r="B112" s="122"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="121"/>
-      <c r="B113" s="122"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="121"/>
-      <c r="B114" s="122"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="121"/>
-      <c r="B115" s="122"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="121"/>
-      <c r="B116" s="122"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="121"/>
-      <c r="B117" s="122"/>
+      <c r="A112" s="118"/>
+      <c r="B112" s="119"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="118"/>
+      <c r="B113" s="119"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="118"/>
+      <c r="B114" s="119"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="118"/>
+      <c r="B115" s="119"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="118"/>
+      <c r="B116" s="119"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="118"/>
+      <c r="B117" s="119"/>
+    </row>
+    <row r="123" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:6" s="62" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="65"/>
+      <c r="C124" s="129" t="s">
+        <v>80</v>
+      </c>
+      <c r="D124" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="E124" s="130">
+        <v>105088.9</v>
+      </c>
+      <c r="F124" s="62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="62" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="65"/>
+      <c r="E125" s="62">
+        <f>E124*1000000</f>
+        <v>105088900000</v>
+      </c>
+      <c r="F125" s="62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" s="62" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="65"/>
+      <c r="D126" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="E126" s="131">
+        <f>(97.3+42.2)</f>
+        <v>139.5</v>
+      </c>
+      <c r="F126" s="62" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="65"/>
+      <c r="E127" s="62">
+        <f>E126*1000000000</f>
+        <v>139500000000</v>
+      </c>
+      <c r="F127" s="62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="65"/>
+    </row>
+    <row r="129" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B129" s="65"/>
+      <c r="E129" s="132">
+        <f>E127/E125</f>
+        <v>1.3274475230019536</v>
+      </c>
+      <c r="F129" s="62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B130" s="65"/>
+    </row>
+    <row r="131" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B131" s="65"/>
+      <c r="D131" s="62" t="str">
+        <f>'Research data'!C7</f>
+        <v>output.passenger_kms</v>
+      </c>
+      <c r="E131" s="62">
+        <f>E129*D28</f>
+        <v>0.60338523772816066</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="65"/>
+    </row>
+    <row r="133" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B133" s="65"/>
+    </row>
+    <row r="134" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B134" s="65"/>
+    </row>
+    <row r="135" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B135" s="65"/>
+    </row>
+    <row r="136" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="65"/>
+    </row>
+    <row r="137" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="65"/>
+    </row>
+    <row r="138" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B138" s="65"/>
+    </row>
+    <row r="139" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B139" s="65"/>
+    </row>
+    <row r="140" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B140" s="65"/>
+    </row>
+    <row r="141" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B141" s="65"/>
+    </row>
+    <row r="142" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="65"/>
+    </row>
+    <row r="143" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B143" s="65"/>
+    </row>
+    <row r="144" spans="2:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B144" s="65"/>
+    </row>
+    <row r="145" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B145" s="65"/>
+    </row>
+    <row r="146" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B146" s="65"/>
+    </row>
+    <row r="147" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B147" s="65"/>
+    </row>
+    <row r="148" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B148" s="65"/>
+    </row>
+    <row r="149" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B149" s="65"/>
+    </row>
+    <row r="150" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B150" s="65"/>
+    </row>
+    <row r="151" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B151" s="65"/>
+    </row>
+    <row r="152" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B152" s="65"/>
+    </row>
+    <row r="153" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B153" s="65"/>
+    </row>
+    <row r="154" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B154" s="65"/>
+    </row>
+    <row r="155" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B155" s="65"/>
+    </row>
+    <row r="156" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B156" s="65"/>
+    </row>
+    <row r="157" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B157" s="65"/>
+    </row>
+    <row r="158" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B158" s="65"/>
+    </row>
+    <row r="159" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B159" s="65"/>
+    </row>
+    <row r="160" spans="2:2" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B160" s="65"/>
+    </row>
+    <row r="161" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B161" s="65"/>
+    </row>
+    <row r="162" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B162" s="65"/>
+    </row>
+    <row r="163" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B163" s="65"/>
+    </row>
+    <row r="164" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B164" s="65"/>
+    </row>
+    <row r="165" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B165" s="65"/>
+    </row>
+    <row r="166" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="65"/>
+    </row>
+    <row r="167" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B167" s="65"/>
+    </row>
+    <row r="168" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B168" s="65"/>
+    </row>
+    <row r="169" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B169" s="65"/>
+    </row>
+    <row r="170" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H170" s="69"/>
+      <c r="I170" s="69"/>
+    </row>
+    <row r="171" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H171" s="69"/>
+      <c r="I171" s="69"/>
+    </row>
+    <row r="172" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H172" s="69"/>
+      <c r="I172" s="69"/>
+    </row>
+    <row r="173" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H173" s="69"/>
+      <c r="I173" s="69"/>
+    </row>
+    <row r="174" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H174" s="69"/>
+      <c r="I174" s="69"/>
+    </row>
+    <row r="175" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H175" s="69"/>
+      <c r="I175" s="69"/>
+    </row>
+    <row r="176" spans="2:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H176" s="69"/>
+      <c r="I176" s="69"/>
+    </row>
+    <row r="177" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H177" s="69"/>
+      <c r="I177" s="69"/>
+    </row>
+    <row r="178" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H178" s="69"/>
+      <c r="I178" s="69"/>
+    </row>
+    <row r="179" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H179" s="69"/>
+      <c r="I179" s="69"/>
+    </row>
+    <row r="180" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H180" s="69"/>
+      <c r="I180" s="69"/>
+    </row>
+    <row r="181" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H181" s="69"/>
+      <c r="I181" s="69"/>
+    </row>
+    <row r="182" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H182" s="69"/>
+      <c r="I182" s="69"/>
+    </row>
+    <row r="183" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H183" s="69"/>
+      <c r="I183" s="69"/>
+    </row>
+    <row r="184" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H184" s="69"/>
+      <c r="I184" s="69"/>
+    </row>
+    <row r="185" spans="8:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H185" s="69"/>
+      <c r="I185" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>